<commit_message>
Propuesta uesta interfaz para agregar datos a la BD
Interfaz gráfica propuesta para llenar la base de datos para el inventario de la UG. Propuesta en HTML, CSS y Javascript, utilizando el framework Materialize y la librería jQuery.
</commit_message>
<xml_diff>
--- a/Base de datos/BD_Inventario_UG.xlsx
+++ b/Base de datos/BD_Inventario_UG.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fire_\Documents\Trabajos\Base de datos\Inventario_UG\Base de datos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99F4E94-65B4-4B8F-8E47-DC00D3B5629F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="23175" windowHeight="9750"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
   <si>
     <t>Objeto</t>
   </si>
@@ -163,16 +157,16 @@
     <t>Copiadora.jpg</t>
   </si>
   <si>
-    <t>Paquete hojas de máquina</t>
-  </si>
-  <si>
-    <t>Scribe</t>
-  </si>
-  <si>
-    <t>BWP-20</t>
-  </si>
-  <si>
-    <t>paquete_hojas.jpg</t>
+    <t>Lámpara fluorescente</t>
+  </si>
+  <si>
+    <t>Philips</t>
+  </si>
+  <si>
+    <t>58081 PIANO</t>
+  </si>
+  <si>
+    <t>lampara.jpg</t>
   </si>
   <si>
     <t>Fibra óptica</t>
@@ -223,7 +217,7 @@
     <t>Investigación</t>
   </si>
   <si>
-    <t>Fibras ópticas</t>
+    <t xml:space="preserve">Tubos de ensayo, fuentes de energía, osciloscopios, generador de funciones, multimetros, </t>
   </si>
   <si>
     <t>Deportes</t>
@@ -232,19 +226,31 @@
     <t>Balones, conos, caminadora, red de portería</t>
   </si>
   <si>
+    <t xml:space="preserve">Mantenimiento </t>
+  </si>
+  <si>
     <t>Electrodomesticos</t>
   </si>
   <si>
     <t>horno micro-ondas, refrijerador, estufa</t>
   </si>
   <si>
-    <t xml:space="preserve">Mantenimiento </t>
-  </si>
-  <si>
     <t xml:space="preserve">Limpieza </t>
   </si>
   <si>
+    <t>Vehículos</t>
+  </si>
+  <si>
+    <t>Carros, motos, lanchas, vicicletas</t>
+  </si>
+  <si>
     <t xml:space="preserve">Activación fisica </t>
+  </si>
+  <si>
+    <t>Herramientas</t>
+  </si>
+  <si>
+    <t>Palas, martillos, taladros, desarmadores</t>
   </si>
   <si>
     <t xml:space="preserve">Recreación </t>
@@ -259,8 +265,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,16 +295,346 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -300,15 +642,260 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -316,42 +903,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="60% - Accent3" xfId="10" builtinId="40"/>
+    <cellStyle name="60% - Accent2" xfId="11" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="12" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="13" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="14" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="15" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="16" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="17" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="19" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="20" builtinId="32"/>
+    <cellStyle name="Bad" xfId="21" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="22" builtinId="23"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Calculation" xfId="24" builtinId="22"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
+    <cellStyle name="Note" xfId="28" builtinId="10"/>
+    <cellStyle name="Hipervínculo visitado" xfId="29" builtinId="9"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18"/>
+    <cellStyle name="Moneda" xfId="33" builtinId="4"/>
+    <cellStyle name="Heading 2" xfId="34" builtinId="17"/>
+    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
+    <cellStyle name="CExplanatory Text" xfId="36" builtinId="53"/>
+    <cellStyle name="Currency [0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="38" builtinId="11"/>
+    <cellStyle name="Comma [0]" xfId="39" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50"/>
+    <cellStyle name="Title" xfId="41" builtinId="15"/>
+    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
+    <cellStyle name="40% - Accent3" xfId="43" builtinId="39"/>
+    <cellStyle name="Linked Cell" xfId="44" builtinId="24"/>
+    <cellStyle name="Accent4" xfId="45" builtinId="41"/>
+    <cellStyle name="Porcentaje" xfId="46" builtinId="5"/>
+    <cellStyle name="Coma" xfId="47" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -609,712 +1243,742 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B2:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.14166666666667" customWidth="1"/>
+    <col min="2" max="2" width="11.5666666666667" customWidth="1"/>
+    <col min="3" max="3" width="13.1416666666667" customWidth="1"/>
+    <col min="4" max="4" width="12.425" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.375" customWidth="1"/>
+    <col min="7" max="7" width="17.25" customWidth="1"/>
+    <col min="8" max="8" width="22.875" customWidth="1"/>
+    <col min="9" max="9" width="17.2833333333333" customWidth="1"/>
+    <col min="10" max="10" width="14.7083333333333" customWidth="1"/>
+    <col min="11" max="11" width="16.8583333333333" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.1416666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="21">
-      <c r="B2" s="7" t="s">
+    <row r="2" ht="19.5" spans="2:12">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="2:13">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:13">
-      <c r="B4" s="2">
+    <row r="4" spans="2:12">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>123</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <v>600</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="11">
         <v>40223</v>
       </c>
       <c r="K4" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:13">
-      <c r="B5" s="2">
+    <row r="5" spans="2:12">
+      <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>7</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>234</v>
       </c>
       <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <v>3500</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="11">
         <v>42118</v>
       </c>
       <c r="K5" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:13">
-      <c r="B6" s="2">
+    <row r="6" spans="2:12">
+      <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>345</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="3">
         <v>150</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="11">
         <v>43132</v>
       </c>
       <c r="K6" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:13">
-      <c r="B7" s="2">
+    <row r="7" spans="2:12">
+      <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>2</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>2</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>456</v>
       </c>
       <c r="F7" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <v>250</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="11" t="s">
         <v>28</v>
       </c>
       <c r="K7" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:13">
-      <c r="B8" s="2">
+    <row r="8" spans="2:12">
+      <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>2</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>4</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>567</v>
       </c>
       <c r="F8" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="3">
         <v>6500</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="11">
         <v>42118</v>
       </c>
       <c r="K8" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:13">
-      <c r="B9" s="2">
+    <row r="9" spans="2:12">
+      <c r="B9" s="3">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="3">
         <v>2</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>678</v>
       </c>
       <c r="F9" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="7">
         <v>12000</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="11">
         <v>43132</v>
       </c>
       <c r="K9" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:13">
-      <c r="B10" s="2">
-        <v>7</v>
-      </c>
-      <c r="C10" s="2">
+    <row r="10" spans="2:12">
+      <c r="B10" s="3">
+        <v>200</v>
+      </c>
+      <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="3">
         <v>6</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>789</v>
       </c>
       <c r="F10" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="3">
         <v>1250</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="11" t="s">
         <v>28</v>
       </c>
       <c r="K10" t="s">
         <v>42</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="2:13">
-      <c r="B11" s="2">
+    <row r="11" spans="2:12">
+      <c r="B11" s="3">
         <v>8</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>2</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="3">
         <v>7</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>890</v>
       </c>
       <c r="F11" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="3">
         <v>6500</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="11">
         <v>43132</v>
       </c>
       <c r="K11" t="s">
         <v>46</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="2:13">
-      <c r="B12" s="2">
+    <row r="12" spans="2:12">
+      <c r="B12" s="3">
         <v>9</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>5</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="3">
         <v>1</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="3">
         <v>450</v>
       </c>
       <c r="F12" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="2">
-        <v>120</v>
-      </c>
-      <c r="H12" s="2" t="s">
+      <c r="G12" s="3">
+        <v>300</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J12" s="5">
-        <v>42118</v>
+      <c r="J12" s="11">
+        <v>43884</v>
       </c>
       <c r="K12" t="s">
         <v>50</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:13">
-      <c r="B13" s="2">
+    <row r="13" spans="2:12">
+      <c r="B13" s="3">
         <v>10</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>3</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="3">
         <v>2</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="3">
         <v>120</v>
       </c>
       <c r="F13" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="3">
         <v>250</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J13" s="11" t="s">
         <v>28</v>
       </c>
       <c r="K13" t="s">
         <v>54</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:13">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="2:13">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="2:13" ht="21">
-      <c r="B16" s="8" t="s">
+    <row r="14" spans="2:12">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" ht="19.5" spans="2:12">
+      <c r="B16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="G16" s="8" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-    </row>
-    <row r="17" spans="2:13">
-      <c r="B17" t="s">
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="B17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="4"/>
-      <c r="G17" t="s">
+      <c r="D17" s="3"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="I17" t="s">
+      <c r="G17" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="J17" s="9" t="s">
+      <c r="H17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="2">
+      <c r="B18" s="3">
         <v>1</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="G18" s="2">
+      <c r="D18" s="6"/>
+      <c r="F18" s="3">
         <v>1</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2" t="s">
+      <c r="G18" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="H18" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="2">
+      <c r="B19" s="3">
         <v>2</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="G19" s="2">
+      <c r="D19" s="6"/>
+      <c r="F19" s="3">
         <v>2</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2" t="s">
+      <c r="G19" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="H19" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="2">
+      <c r="B20" s="3">
         <v>3</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="G20" s="2">
+      <c r="D20" s="6"/>
+      <c r="F20" s="3">
         <v>3</v>
       </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2" t="s">
+      <c r="G20" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="H20" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="2">
+      <c r="B21" s="3">
         <v>4</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="G21" s="2">
+      <c r="D21" s="6"/>
+      <c r="F21" s="3">
         <v>4</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2" t="s">
+      <c r="G21" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="H21" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
     </row>
     <row r="22" spans="2:13">
-      <c r="B22" s="2">
+      <c r="B22" s="3">
         <v>5</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="F22" s="3">
+        <v>5</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="G22" s="2">
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+    </row>
+    <row r="23" spans="2:13">
+      <c r="B23" s="3">
         <v>6</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-    </row>
-    <row r="23" spans="2:13">
-      <c r="B23" s="2">
+      <c r="C23" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="F23" s="5">
         <v>6</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="10"/>
+      <c r="G23" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
     </row>
     <row r="24" spans="2:13">
-      <c r="B24" s="2">
+      <c r="B24" s="3">
         <v>7</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
+      <c r="C24" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="F24" s="5">
+        <v>7</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
     </row>
     <row r="25" spans="2:13">
-      <c r="B25" s="2">
+      <c r="B25" s="3">
         <v>8</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
+      <c r="C25" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
     </row>
     <row r="26" spans="2:13">
-      <c r="B26" s="2">
+      <c r="B26" s="3">
         <v>9</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="10"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
+      <c r="C26" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="2">
+      <c r="B27" s="3">
         <v>10</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="10"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-    </row>
-    <row r="28" spans="2:13">
-      <c r="B28" s="2"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
+      <c r="C27" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="3"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="H26:M26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="J27:M27"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="G16:M16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="J17:M17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modificación de la vista para las categorías y finalidad
</commit_message>
<xml_diff>
--- a/Base de datos/BD_Inventario_UG.xlsx
+++ b/Base de datos/BD_Inventario_UG.xlsx
@@ -305,13 +305,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -334,30 +327,22 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -380,14 +365,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -411,7 +388,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -425,14 +433,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -449,6 +449,132 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -461,175 +587,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -648,15 +648,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,17 +676,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -740,144 +725,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -890,7 +890,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -907,19 +907,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1321,7 +1312,7 @@
       <c r="L3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1350,7 +1341,7 @@
       <c r="I4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="8">
         <v>40223</v>
       </c>
       <c r="K4" t="s">
@@ -1385,7 +1376,7 @@
       <c r="I5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="8">
         <v>42118</v>
       </c>
       <c r="K5" t="s">
@@ -1420,7 +1411,7 @@
       <c r="I6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="8">
         <v>43132</v>
       </c>
       <c r="K6" t="s">
@@ -1455,7 +1446,7 @@
       <c r="I7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="8" t="s">
         <v>28</v>
       </c>
       <c r="K7" t="s">
@@ -1490,7 +1481,7 @@
       <c r="I8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="8">
         <v>42118</v>
       </c>
       <c r="K8" t="s">
@@ -1516,16 +1507,16 @@
       <c r="F9" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>12000</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="6" t="s">
         <v>36</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="8">
         <v>43132</v>
       </c>
       <c r="K9" t="s">
@@ -1560,7 +1551,7 @@
       <c r="I10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="8" t="s">
         <v>28</v>
       </c>
       <c r="K10" t="s">
@@ -1595,7 +1586,7 @@
       <c r="I11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="8">
         <v>43132</v>
       </c>
       <c r="K11" t="s">
@@ -1630,7 +1621,7 @@
       <c r="I12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="8">
         <v>43884</v>
       </c>
       <c r="K12" t="s">
@@ -1665,7 +1656,7 @@
       <c r="I13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="8" t="s">
         <v>28</v>
       </c>
       <c r="K13" t="s">
@@ -1713,18 +1704,18 @@
       <c r="L16" s="4"/>
     </row>
     <row r="17" spans="2:12">
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="5" t="s">
+      <c r="E17" s="7"/>
+      <c r="F17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="3" t="s">
         <v>58</v>
       </c>
       <c r="H17" s="3" t="s">
@@ -1738,217 +1729,217 @@
       <c r="B18" s="3">
         <v>1</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="5"/>
       <c r="F18" s="3">
         <v>1</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
     </row>
     <row r="19" spans="2:13">
       <c r="B19" s="3">
         <v>2</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="6"/>
+      <c r="D19" s="5"/>
       <c r="F19" s="3">
         <v>2</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
     </row>
     <row r="20" spans="2:13">
       <c r="B20" s="3">
         <v>3</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="5"/>
       <c r="F20" s="3">
         <v>3</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
     </row>
     <row r="21" spans="2:13">
       <c r="B21" s="3">
         <v>4</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="6"/>
+      <c r="D21" s="5"/>
       <c r="F21" s="3">
         <v>4</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
     </row>
     <row r="22" spans="2:13">
       <c r="B22" s="3">
         <v>5</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="5"/>
       <c r="F22" s="3">
         <v>5</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
     </row>
     <row r="23" spans="2:13">
       <c r="B23" s="3">
         <v>6</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="F23" s="5">
+      <c r="D23" s="5"/>
+      <c r="F23" s="3">
         <v>6</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
     </row>
     <row r="24" spans="2:13">
       <c r="B24" s="3">
         <v>7</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="F24" s="5">
+      <c r="D24" s="5"/>
+      <c r="F24" s="3">
         <v>7</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
     </row>
     <row r="25" spans="2:13">
       <c r="B25" s="3">
         <v>8</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="D25" s="5"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
     </row>
     <row r="26" spans="2:13">
       <c r="B26" s="3">
         <v>9</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
+      <c r="D26" s="5"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
     </row>
     <row r="27" spans="2:13">
       <c r="B27" s="3">
         <v>10</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D27" s="6"/>
+      <c r="D27" s="5"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="3"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="25">

</xml_diff>

<commit_message>
Nuevo archivo y modificaciones
Archivo de recursos bajo resguardo de Goevanni y tabla de categorías y sub-categorias
</commit_message>
<xml_diff>
--- a/Base de datos/BD_Inventario_UG.xlsx
+++ b/Base de datos/BD_Inventario_UG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23175" windowHeight="9750"/>
+    <workbookView windowWidth="23175" windowHeight="9075"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="106">
   <si>
     <t>Objeto</t>
   </si>
@@ -260,6 +260,78 @@
   </si>
   <si>
     <t xml:space="preserve">Cocinar </t>
+  </si>
+  <si>
+    <t>Sub-Categorias</t>
+  </si>
+  <si>
+    <t>Sub-división</t>
+  </si>
+  <si>
+    <t>ID_Subcategoria</t>
+  </si>
+  <si>
+    <t>ID_Subdivision</t>
+  </si>
+  <si>
+    <t>Computación</t>
+  </si>
+  <si>
+    <t>Toda clase de computadoras</t>
+  </si>
+  <si>
+    <t>Desktop</t>
+  </si>
+  <si>
+    <t>Computadora de escritorio convencional con CPU</t>
+  </si>
+  <si>
+    <t>Impresoras</t>
+  </si>
+  <si>
+    <t>Tipos de impresoras: tinta, láser o 3D</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>Computadora portatil en las categorias: laptop y ultrabook</t>
+  </si>
+  <si>
+    <t>Drones</t>
+  </si>
+  <si>
+    <t>Drones programables, modular, etc</t>
+  </si>
+  <si>
+    <t>Servidor</t>
+  </si>
+  <si>
+    <t>Computadora especializada para el alto rendimiento</t>
+  </si>
+  <si>
+    <t>Oficina</t>
+  </si>
+  <si>
+    <t>Muebles para oficinas</t>
+  </si>
+  <si>
+    <t>Mini-PC</t>
+  </si>
+  <si>
+    <t>Computadora de formato pequeño tipo: Raspberry PI, Intel NUC o Apple Mini</t>
+  </si>
+  <si>
+    <t>Salas</t>
+  </si>
+  <si>
+    <t>Muebles para salas</t>
+  </si>
+  <si>
+    <t>All-In-One</t>
+  </si>
+  <si>
+    <t>Computadora en la cual el CPU está embebido en un case junto al monitor</t>
   </si>
 </sst>
 </file>
@@ -267,9 +339,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -296,23 +368,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -341,8 +398,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -350,7 +430,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -365,15 +445,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -388,14 +467,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -409,17 +481,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -434,7 +506,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -449,187 +521,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,15 +724,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -676,15 +739,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -696,6 +750,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -726,17 +795,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -745,109 +817,109 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -856,28 +928,28 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -886,11 +958,11 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -909,14 +981,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1240,7 +1336,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:M28"/>
+  <dimension ref="B2:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1249,18 +1345,18 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="2.14166666666667" customWidth="1"/>
-    <col min="2" max="2" width="11.5666666666667" customWidth="1"/>
+    <col min="2" max="2" width="15.625" customWidth="1"/>
     <col min="3" max="3" width="13.1416666666667" customWidth="1"/>
     <col min="4" max="4" width="12.425" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="23.375" customWidth="1"/>
+    <col min="6" max="6" width="22.375" customWidth="1"/>
     <col min="7" max="7" width="17.25" customWidth="1"/>
-    <col min="8" max="8" width="22.875" customWidth="1"/>
-    <col min="9" max="9" width="17.2833333333333" customWidth="1"/>
-    <col min="10" max="10" width="14.7083333333333" customWidth="1"/>
-    <col min="11" max="11" width="16.8583333333333" customWidth="1"/>
+    <col min="8" max="8" width="14.875" customWidth="1"/>
+    <col min="9" max="9" width="13.125" customWidth="1"/>
+    <col min="10" max="10" width="15.625" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="12.1416666666667" customWidth="1"/>
+    <col min="13" max="13" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" ht="19.5" spans="2:12">
@@ -1312,7 +1408,7 @@
       <c r="L3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="17" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1341,7 +1437,7 @@
       <c r="I4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="13">
         <v>40223</v>
       </c>
       <c r="K4" t="s">
@@ -1376,7 +1472,7 @@
       <c r="I5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="13">
         <v>42118</v>
       </c>
       <c r="K5" t="s">
@@ -1411,7 +1507,7 @@
       <c r="I6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="13">
         <v>43132</v>
       </c>
       <c r="K6" t="s">
@@ -1446,7 +1542,7 @@
       <c r="I7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="13" t="s">
         <v>28</v>
       </c>
       <c r="K7" t="s">
@@ -1481,7 +1577,7 @@
       <c r="I8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="13">
         <v>42118</v>
       </c>
       <c r="K8" t="s">
@@ -1507,16 +1603,16 @@
       <c r="F9" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="9">
         <v>12000</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="9" t="s">
         <v>36</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="13">
         <v>43132</v>
       </c>
       <c r="K9" t="s">
@@ -1551,7 +1647,7 @@
       <c r="I10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="13" t="s">
         <v>28</v>
       </c>
       <c r="K10" t="s">
@@ -1586,7 +1682,7 @@
       <c r="I11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="13">
         <v>43132</v>
       </c>
       <c r="K11" t="s">
@@ -1621,7 +1717,7 @@
       <c r="I12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="13">
         <v>43884</v>
       </c>
       <c r="K12" t="s">
@@ -1656,7 +1752,7 @@
       <c r="I13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="13" t="s">
         <v>28</v>
       </c>
       <c r="K13" t="s">
@@ -1711,7 +1807,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="7"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="3" t="s">
         <v>57</v>
       </c>
@@ -1854,14 +1950,14 @@
       <c r="G23" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H23" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
     </row>
     <row r="24" spans="2:13">
       <c r="B24" s="3">
@@ -1920,7 +2016,7 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
     </row>
-    <row r="27" spans="2:13">
+    <row r="27" spans="2:4">
       <c r="B27" s="3">
         <v>10</v>
       </c>
@@ -1928,21 +2024,263 @@
         <v>81</v>
       </c>
       <c r="D27" s="5"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="3"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
+    <row r="29" ht="19.5" spans="2:10">
+      <c r="B29" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="G29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+    </row>
+    <row r="30" spans="2:15">
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" t="s">
+        <v>85</v>
+      </c>
+      <c r="H30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+    </row>
+    <row r="31" spans="2:15">
+      <c r="B31" s="8">
+        <v>1</v>
+      </c>
+      <c r="C31" s="8">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="8">
+        <v>1</v>
+      </c>
+      <c r="H31" s="8">
+        <v>1</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+    </row>
+    <row r="32" spans="2:15">
+      <c r="B32" s="8">
+        <v>2</v>
+      </c>
+      <c r="C32" s="8">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="8">
+        <v>2</v>
+      </c>
+      <c r="H32" s="8">
+        <v>1</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+    </row>
+    <row r="33" spans="2:15">
+      <c r="B33" s="8">
+        <v>3</v>
+      </c>
+      <c r="C33" s="8">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="8">
+        <v>3</v>
+      </c>
+      <c r="H33" s="8">
+        <v>1</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+    </row>
+    <row r="34" spans="2:15">
+      <c r="B34" s="8">
+        <v>4</v>
+      </c>
+      <c r="C34" s="8">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F34" s="12"/>
+      <c r="G34" s="8">
+        <v>4</v>
+      </c>
+      <c r="H34" s="8">
+        <v>1</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+    </row>
+    <row r="35" spans="2:15">
+      <c r="B35" s="8">
+        <v>5</v>
+      </c>
+      <c r="C35" s="8">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="8">
+        <v>5</v>
+      </c>
+      <c r="H35" s="8">
+        <v>1</v>
+      </c>
+      <c r="I35" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+    </row>
+    <row r="36" spans="2:15">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="G36" s="8">
+        <v>6</v>
+      </c>
+      <c r="H36" s="8"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+    </row>
+    <row r="37" spans="2:11">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="G37" s="8">
+        <v>7</v>
+      </c>
+      <c r="H37" s="8"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+    </row>
+    <row r="38" spans="7:8">
+      <c r="G38" s="8">
+        <v>8</v>
+      </c>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="7:8">
+      <c r="G39" s="8">
+        <v>9</v>
+      </c>
+      <c r="H39" s="8"/>
+    </row>
+    <row r="40" spans="7:8">
+      <c r="G40" s="8">
+        <v>10</v>
+      </c>
+      <c r="H40" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="38">
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="F16:H16"/>
@@ -1966,8 +2304,21 @@
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="H26:M26"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="J27:M27"/>
     <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="J30:O30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="J31:O31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="J32:O32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="J33:O33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="J34:O34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="J35:O35"/>
+    <mergeCell ref="J36:O36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>